<commit_message>
Update of 'other publication formats' OA and licenses charts
- Added WE3 institution to OA;
- Added filter for insitutions;
- Applyed the year slider;

TODO:
- WE1 institution;
- Percentage counting for OA and licenses
</commit_message>
<xml_diff>
--- a/dashboard/data/we2_alt_publ3.xlsx
+++ b/dashboard/data/we2_alt_publ3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaatn\Documents\R\BIH Projects\geoscience-dashboard-ana-copy\dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{532847B5-1304-4754-84B0-078A1FF4D016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BBEA1D7-E8C9-433A-827E-6189E68C599B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2016" sheetId="1" r:id="rId1"/>
@@ -995,7 +995,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1091,6 +1091,10 @@
     <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -1321,8 +1325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
@@ -1331,8 +1335,9 @@
     <col min="2" max="2" width="30.19921875" customWidth="1"/>
     <col min="3" max="3" width="11" style="2"/>
     <col min="4" max="4" width="11" style="1"/>
-    <col min="5" max="9" width="0" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="0" hidden="1" customWidth="1"/>
+    <col min="5" max="8" width="11.19921875" customWidth="1"/>
+    <col min="9" max="9" width="11.19921875" style="59" customWidth="1"/>
+    <col min="11" max="11" width="11.19921875" customWidth="1"/>
     <col min="12" max="12" width="11" style="2"/>
     <col min="13" max="13" width="11" style="1"/>
     <col min="14" max="14" width="0" hidden="1" customWidth="1"/>
@@ -1363,7 +1368,7 @@
       <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="57" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="5" t="s">
@@ -1447,7 +1452,7 @@
       <c r="H2" s="9" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I2" s="9" t="e">
+      <c r="I2" s="11" t="e">
         <v>#N/A</v>
       </c>
       <c r="J2" s="9" t="b">
@@ -1615,7 +1620,7 @@
       <c r="H4" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="I4" s="9" t="e">
+      <c r="I4" s="11" t="e">
         <v>#N/A</v>
       </c>
       <c r="J4" s="9" t="b">
@@ -1699,7 +1704,7 @@
       <c r="H5" s="9" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I5" s="9" t="e">
+      <c r="I5" s="11" t="e">
         <v>#N/A</v>
       </c>
       <c r="J5" s="9" t="b">
@@ -1783,7 +1788,7 @@
       <c r="H6" s="9" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I6" s="9" t="e">
+      <c r="I6" s="11" t="e">
         <v>#N/A</v>
       </c>
       <c r="J6" s="9" t="b">
@@ -1867,7 +1872,7 @@
       <c r="H7" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I7" s="15" t="e">
+      <c r="I7" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J7" s="15" t="b">
@@ -1952,7 +1957,7 @@
       <c r="H8" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I8" s="15" t="e">
+      <c r="I8" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J8" s="15" t="b">
@@ -2037,7 +2042,7 @@
       <c r="H9" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I9" s="15" t="e">
+      <c r="I9" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J9" s="15" t="b">
@@ -2122,7 +2127,7 @@
       <c r="H10" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I10" s="15" t="e">
+      <c r="I10" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J10" s="15" t="b">
@@ -2207,7 +2212,7 @@
       <c r="H11" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I11" s="15" t="e">
+      <c r="I11" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J11" s="15" t="b">
@@ -2292,7 +2297,7 @@
       <c r="H12" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I12" s="15" t="e">
+      <c r="I12" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J12" s="15" t="b">
@@ -2375,7 +2380,7 @@
       <c r="H13" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I13" s="15" t="e">
+      <c r="I13" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J13" s="15" t="b">
@@ -2460,7 +2465,7 @@
       <c r="H14" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I14" s="15" t="e">
+      <c r="I14" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J14" s="15" t="b">
@@ -2545,7 +2550,7 @@
       <c r="H15" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I15" s="15" t="e">
+      <c r="I15" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J15" s="15" t="b">
@@ -2630,7 +2635,7 @@
       <c r="H16" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I16" s="15" t="e">
+      <c r="I16" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J16" s="15" t="b">
@@ -2717,7 +2722,7 @@
       <c r="H17" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I17" s="15" t="e">
+      <c r="I17" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J17" s="15" t="b">
@@ -2802,7 +2807,7 @@
       <c r="H18" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I18" s="15" t="e">
+      <c r="I18" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J18" s="15" t="b">
@@ -2885,8 +2890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AG13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
@@ -2894,7 +2899,8 @@
     <col min="1" max="1" width="58" style="1" customWidth="1"/>
     <col min="2" max="2" width="32.09765625" customWidth="1"/>
     <col min="3" max="3" width="22.296875" style="2" customWidth="1"/>
-    <col min="5" max="9" width="10.69921875" customWidth="1"/>
+    <col min="5" max="8" width="10.69921875" customWidth="1"/>
+    <col min="9" max="9" width="10.69921875" style="59" customWidth="1"/>
     <col min="10" max="10" width="11" style="2"/>
     <col min="11" max="11" width="10.69921875" customWidth="1"/>
     <col min="13" max="13" width="11" style="2"/>
@@ -2925,7 +2931,7 @@
       <c r="H1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="60" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="22" t="s">
@@ -3099,7 +3105,7 @@
       <c r="H3" s="9" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I3" s="9" t="e">
+      <c r="I3" s="11" t="e">
         <v>#N/A</v>
       </c>
       <c r="J3" s="10" t="b">
@@ -3187,7 +3193,7 @@
       <c r="H4" s="9" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I4" s="9" t="e">
+      <c r="I4" s="11" t="e">
         <v>#N/A</v>
       </c>
       <c r="J4" s="10" t="b">
@@ -3273,7 +3279,7 @@
       <c r="H5" s="9" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I5" s="9" t="e">
+      <c r="I5" s="11" t="e">
         <v>#N/A</v>
       </c>
       <c r="J5" s="10" t="b">
@@ -3361,7 +3367,7 @@
       <c r="H6" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I6" s="15" t="e">
+      <c r="I6" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J6" s="14" t="b">
@@ -3444,7 +3450,7 @@
       <c r="H7" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I7" s="15" t="e">
+      <c r="I7" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J7" s="14" t="b">
@@ -3529,7 +3535,7 @@
       <c r="H8" s="9" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I8" s="9" t="e">
+      <c r="I8" s="11" t="e">
         <v>#N/A</v>
       </c>
       <c r="J8" s="10" t="b">
@@ -3614,7 +3620,7 @@
       <c r="H9" s="9" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I9" s="9" t="e">
+      <c r="I9" s="11" t="e">
         <v>#N/A</v>
       </c>
       <c r="J9" s="10" t="b">
@@ -3697,7 +3703,7 @@
       <c r="H10" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I10" s="15" t="e">
+      <c r="I10" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J10" s="14" t="b">
@@ -3782,7 +3788,7 @@
       <c r="H11" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I11" s="15" t="e">
+      <c r="I11" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J11" s="14" t="b">
@@ -3865,7 +3871,7 @@
       <c r="H12" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I12" s="15" t="e">
+      <c r="I12" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J12" s="14" t="b">
@@ -3948,7 +3954,7 @@
       <c r="H13" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I13" s="15" t="e">
+      <c r="I13" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J13" s="14" t="b">
@@ -4028,14 +4034,15 @@
   <dimension ref="A1:AG12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="59" customWidth="1"/>
     <col min="2" max="2" width="19.19921875" customWidth="1"/>
-    <col min="5" max="9" width="11" customWidth="1"/>
+    <col min="5" max="8" width="11" customWidth="1"/>
+    <col min="9" max="9" width="11" style="59" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
     <col min="12" max="12" width="13.296875" style="2" customWidth="1"/>
     <col min="13" max="13" width="13" customWidth="1"/>
@@ -4072,7 +4079,7 @@
       <c r="H1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="60" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="21" t="s">
@@ -4158,7 +4165,7 @@
       <c r="H2" s="25" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I2" s="25" t="e">
+      <c r="I2" s="27" t="e">
         <v>#N/A</v>
       </c>
       <c r="J2" s="25" t="b">
@@ -4244,7 +4251,7 @@
       <c r="H3" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I3" s="15" t="e">
+      <c r="I3" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J3" s="15" t="b">
@@ -4331,7 +4338,7 @@
       <c r="H4" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I4" s="15" t="e">
+      <c r="I4" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J4" s="15" t="b">
@@ -4418,7 +4425,7 @@
       <c r="H5" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I5" s="15" t="e">
+      <c r="I5" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J5" s="15" t="b">
@@ -4505,7 +4512,7 @@
       <c r="H6" s="9" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I6" s="9" t="e">
+      <c r="I6" s="11" t="e">
         <v>#N/A</v>
       </c>
       <c r="J6" s="9" t="b">
@@ -4592,7 +4599,7 @@
       <c r="H7" s="9" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I7" s="9" t="e">
+      <c r="I7" s="11" t="e">
         <v>#N/A</v>
       </c>
       <c r="J7" s="9" t="b">
@@ -4681,7 +4688,7 @@
       <c r="H8" s="9" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I8" s="9" t="e">
+      <c r="I8" s="11" t="e">
         <v>#N/A</v>
       </c>
       <c r="J8" s="9" t="b">
@@ -4767,7 +4774,7 @@
       <c r="H9" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I9" s="15" t="e">
+      <c r="I9" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J9" s="15" t="b">
@@ -4852,7 +4859,7 @@
       <c r="H10" s="9" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I10" s="9" t="e">
+      <c r="I10" s="11" t="e">
         <v>#N/A</v>
       </c>
       <c r="J10" s="9" t="b">
@@ -4936,7 +4943,7 @@
       <c r="H11" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I11" s="15" t="e">
+      <c r="I11" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J11" s="15" t="b">
@@ -5022,7 +5029,7 @@
       <c r="H12" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I12" s="15" t="e">
+      <c r="I12" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J12" s="15" t="b">
@@ -5106,7 +5113,7 @@
   <dimension ref="A1:AG11"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -5114,7 +5121,8 @@
     <col min="1" max="1" width="49.296875" customWidth="1"/>
     <col min="2" max="2" width="31" style="2" customWidth="1"/>
     <col min="4" max="4" width="11" style="2"/>
-    <col min="5" max="9" width="11" customWidth="1"/>
+    <col min="5" max="8" width="11" customWidth="1"/>
+    <col min="9" max="9" width="11" style="59" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
     <col min="12" max="12" width="11" style="2"/>
   </cols>
@@ -5144,7 +5152,7 @@
       <c r="H1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="60" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="21" t="s">
@@ -5230,7 +5238,7 @@
       <c r="H2" s="25" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I2" s="25" t="e">
+      <c r="I2" s="27" t="e">
         <v>#N/A</v>
       </c>
       <c r="J2" s="25" t="b">
@@ -5400,7 +5408,7 @@
       <c r="H4" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I4" s="15" t="e">
+      <c r="I4" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J4" s="15" t="b">
@@ -5482,7 +5490,7 @@
       <c r="H5" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I5" s="15" t="e">
+      <c r="I5" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J5" s="15" t="b">
@@ -5566,7 +5574,7 @@
       <c r="H6" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I6" s="15" t="e">
+      <c r="I6" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J6" s="15" t="b">
@@ -5650,7 +5658,7 @@
       <c r="H7" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I7" s="15" t="e">
+      <c r="I7" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J7" s="15" t="b">
@@ -5736,7 +5744,7 @@
       <c r="H8" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I8" s="15" t="e">
+      <c r="I8" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J8" s="15" t="b">
@@ -5822,7 +5830,7 @@
       <c r="H9" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I9" s="15" t="e">
+      <c r="I9" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J9" s="15" t="b">
@@ -5906,7 +5914,7 @@
       <c r="H10" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I10" s="15" t="e">
+      <c r="I10" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J10" s="15" t="b">
@@ -5986,7 +5994,7 @@
       <c r="H11" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I11" s="15" t="e">
+      <c r="I11" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J11" s="15" t="b">
@@ -6064,13 +6072,14 @@
   <dimension ref="A1:AG6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="49.5" customWidth="1"/>
-    <col min="5" max="9" width="11" customWidth="1"/>
+    <col min="5" max="8" width="11" customWidth="1"/>
+    <col min="9" max="9" width="11" style="59" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6099,7 +6108,7 @@
       <c r="H1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="60" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="21" t="s">
@@ -6187,7 +6196,7 @@
       <c r="H2" s="25" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I2" s="25" t="e">
+      <c r="I2" s="27" t="e">
         <v>#N/A</v>
       </c>
       <c r="J2" s="25" t="b">
@@ -6273,7 +6282,7 @@
       <c r="H3" s="9" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I3" s="9" t="e">
+      <c r="I3" s="11" t="e">
         <v>#N/A</v>
       </c>
       <c r="J3" s="9" t="b">
@@ -6359,7 +6368,7 @@
       <c r="H4" s="9" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I4" s="9" t="e">
+      <c r="I4" s="11" t="e">
         <v>#N/A</v>
       </c>
       <c r="J4" s="9" t="b">
@@ -6447,7 +6456,7 @@
       <c r="H5" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I5" s="15" t="e">
+      <c r="I5" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J5" s="15" t="b">
@@ -6536,7 +6545,7 @@
       <c r="H6" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I6" s="15" t="e">
+      <c r="I6" s="58" t="e">
         <v>#N/A</v>
       </c>
       <c r="J6" s="15" t="b">
@@ -6618,8 +6627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AF15"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.4"/>

</xml_diff>